<commit_message>
Modul Informasi : Membuat tampilan Detail slip gaji
</commit_message>
<xml_diff>
--- a/tests/Form Import Gaji.xlsx
+++ b/tests/Form Import Gaji.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Gaji Dasar</t>
   </si>
@@ -59,15 +59,6 @@
     <t>Rapel</t>
   </si>
   <si>
-    <t>Bpjs Tenaga Kerja</t>
-  </si>
-  <si>
-    <t>Bpjs Kesehatan</t>
-  </si>
-  <si>
-    <t>Bpjs Dana Pensiun</t>
-  </si>
-  <si>
     <t>Komunikasi</t>
   </si>
   <si>
@@ -102,6 +93,24 @@
   </si>
   <si>
     <t>Potongan Lain 3</t>
+  </si>
+  <si>
+    <t>Total Pendapatan</t>
+  </si>
+  <si>
+    <t>Total Potongan</t>
+  </si>
+  <si>
+    <t>Total Takehome</t>
+  </si>
+  <si>
+    <t>BPJS Tenaga Kerja</t>
+  </si>
+  <si>
+    <t>BPJS Kesehatan</t>
+  </si>
+  <si>
+    <t>Dana Pensiun</t>
   </si>
 </sst>
 </file>
@@ -419,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,11 +454,14 @@
     <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="15" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -485,244 +497,280 @@
         <v>10</v>
       </c>
       <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" t="s">
+        <v>11</v>
+      </c>
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="U1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="W1" t="s">
+        <v>23</v>
+      </c>
+      <c r="X1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>100000</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2">
+        <v>100000</v>
+      </c>
+      <c r="E2">
+        <v>100000</v>
+      </c>
+      <c r="F2">
+        <v>100000</v>
+      </c>
+      <c r="G2">
+        <v>100000</v>
+      </c>
+      <c r="H2">
+        <v>100000</v>
+      </c>
+      <c r="I2">
+        <v>100000</v>
+      </c>
+      <c r="J2">
+        <v>100000</v>
+      </c>
+      <c r="K2">
+        <v>100000</v>
+      </c>
+      <c r="L2">
+        <v>100000</v>
+      </c>
+      <c r="M2">
+        <v>100000</v>
+      </c>
+      <c r="N2">
+        <v>100000</v>
+      </c>
+      <c r="O2">
+        <v>100000</v>
+      </c>
+      <c r="P2">
+        <v>100000</v>
+      </c>
+      <c r="Q2">
+        <v>100000</v>
+      </c>
+      <c r="R2">
+        <v>100000</v>
+      </c>
+      <c r="S2">
+        <v>100000</v>
+      </c>
+      <c r="T2">
+        <v>100000</v>
+      </c>
+      <c r="U2">
+        <v>100000</v>
+      </c>
+      <c r="V2">
+        <v>100000</v>
+      </c>
+      <c r="W2">
+        <v>14000000</v>
+      </c>
+      <c r="X2">
+        <v>7000000</v>
+      </c>
+      <c r="Y2">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>100000</v>
+      </c>
+      <c r="C3">
+        <v>100000</v>
+      </c>
+      <c r="D3">
+        <v>100000</v>
+      </c>
+      <c r="E3">
+        <v>100000</v>
+      </c>
+      <c r="F3">
+        <v>100000</v>
+      </c>
+      <c r="G3">
+        <v>100000</v>
+      </c>
+      <c r="H3">
+        <v>100000</v>
+      </c>
+      <c r="I3">
+        <v>100000</v>
+      </c>
+      <c r="J3">
+        <v>100000</v>
+      </c>
+      <c r="K3">
+        <v>100000</v>
+      </c>
+      <c r="L3">
+        <v>100000</v>
+      </c>
+      <c r="M3">
+        <v>100000</v>
+      </c>
+      <c r="N3">
+        <v>100000</v>
+      </c>
+      <c r="O3">
+        <v>100000</v>
+      </c>
+      <c r="P3">
+        <v>100000</v>
+      </c>
+      <c r="Q3">
+        <v>100000</v>
+      </c>
+      <c r="R3">
+        <v>100000</v>
+      </c>
+      <c r="S3">
+        <v>100000</v>
+      </c>
+      <c r="T3">
+        <v>100000</v>
+      </c>
+      <c r="U3">
+        <v>100000</v>
+      </c>
+      <c r="V3">
+        <v>100000</v>
+      </c>
+      <c r="W3">
+        <v>15000000</v>
+      </c>
+      <c r="X3">
+        <v>6000000</v>
+      </c>
+      <c r="Y3">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>100000</v>
+      </c>
+      <c r="C4">
+        <v>100000</v>
+      </c>
+      <c r="D4">
+        <v>100000</v>
+      </c>
+      <c r="E4">
+        <v>100000</v>
+      </c>
+      <c r="F4">
+        <v>100000</v>
+      </c>
+      <c r="G4">
+        <v>100000</v>
+      </c>
+      <c r="H4">
+        <v>100000</v>
+      </c>
+      <c r="I4">
+        <v>100000</v>
+      </c>
+      <c r="J4">
+        <v>100000</v>
+      </c>
+      <c r="K4">
+        <v>100000</v>
+      </c>
+      <c r="L4">
+        <v>100000</v>
+      </c>
+      <c r="M4">
+        <v>100000</v>
+      </c>
+      <c r="N4">
+        <v>100000</v>
+      </c>
+      <c r="O4">
+        <v>100000</v>
+      </c>
+      <c r="P4">
+        <v>100000</v>
+      </c>
+      <c r="Q4">
+        <v>100000</v>
+      </c>
+      <c r="R4">
+        <v>100000</v>
+      </c>
+      <c r="S4">
+        <v>100000</v>
+      </c>
+      <c r="T4">
+        <v>100000</v>
+      </c>
+      <c r="U4">
+        <v>100000</v>
+      </c>
+      <c r="V4">
+        <v>100000</v>
+      </c>
+      <c r="W4">
+        <v>16000000</v>
+      </c>
+      <c r="X4">
+        <v>5000000</v>
+      </c>
+      <c r="Y4">
+        <v>9000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" t="s">
-        <v>24</v>
-      </c>
-      <c r="V1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2">
-        <v>100000</v>
-      </c>
-      <c r="C2">
-        <v>100000</v>
-      </c>
-      <c r="D2">
-        <v>100000</v>
-      </c>
-      <c r="E2">
-        <v>100000</v>
-      </c>
-      <c r="F2">
-        <v>100000</v>
-      </c>
-      <c r="G2">
-        <v>100000</v>
-      </c>
-      <c r="H2">
-        <v>100000</v>
-      </c>
-      <c r="I2">
-        <v>100000</v>
-      </c>
-      <c r="J2">
-        <v>100000</v>
-      </c>
-      <c r="K2">
-        <v>100000</v>
-      </c>
-      <c r="L2">
-        <v>100000</v>
-      </c>
-      <c r="M2">
-        <v>100000</v>
-      </c>
-      <c r="N2">
-        <v>100000</v>
-      </c>
-      <c r="O2">
-        <v>100000</v>
-      </c>
-      <c r="P2">
-        <v>100000</v>
-      </c>
-      <c r="Q2">
-        <v>100000</v>
-      </c>
-      <c r="R2">
-        <v>100000</v>
-      </c>
-      <c r="S2">
-        <v>100000</v>
-      </c>
-      <c r="T2">
-        <v>100000</v>
-      </c>
-      <c r="U2">
-        <v>100000</v>
-      </c>
-      <c r="V2">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3">
-        <v>100000</v>
-      </c>
-      <c r="C3">
-        <v>100000</v>
-      </c>
-      <c r="D3">
-        <v>100000</v>
-      </c>
-      <c r="E3">
-        <v>100000</v>
-      </c>
-      <c r="F3">
-        <v>100000</v>
-      </c>
-      <c r="G3">
-        <v>100000</v>
-      </c>
-      <c r="H3">
-        <v>100000</v>
-      </c>
-      <c r="I3">
-        <v>100000</v>
-      </c>
-      <c r="J3">
-        <v>100000</v>
-      </c>
-      <c r="K3">
-        <v>100000</v>
-      </c>
-      <c r="L3">
-        <v>100000</v>
-      </c>
-      <c r="M3">
-        <v>100000</v>
-      </c>
-      <c r="N3">
-        <v>100000</v>
-      </c>
-      <c r="O3">
-        <v>100000</v>
-      </c>
-      <c r="P3">
-        <v>100000</v>
-      </c>
-      <c r="Q3">
-        <v>100000</v>
-      </c>
-      <c r="R3">
-        <v>100000</v>
-      </c>
-      <c r="S3">
-        <v>100000</v>
-      </c>
-      <c r="T3">
-        <v>100000</v>
-      </c>
-      <c r="U3">
-        <v>100000</v>
-      </c>
-      <c r="V3">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>100000</v>
-      </c>
-      <c r="C4">
-        <v>100000</v>
-      </c>
-      <c r="D4">
-        <v>100000</v>
-      </c>
-      <c r="E4">
-        <v>100000</v>
-      </c>
-      <c r="F4">
-        <v>100000</v>
-      </c>
-      <c r="G4">
-        <v>100000</v>
-      </c>
-      <c r="H4">
-        <v>100000</v>
-      </c>
-      <c r="I4">
-        <v>100000</v>
-      </c>
-      <c r="J4">
-        <v>100000</v>
-      </c>
-      <c r="K4">
-        <v>100000</v>
-      </c>
-      <c r="L4">
-        <v>100000</v>
-      </c>
-      <c r="M4">
-        <v>100000</v>
-      </c>
-      <c r="N4">
-        <v>100000</v>
-      </c>
-      <c r="O4">
-        <v>100000</v>
-      </c>
-      <c r="P4">
-        <v>100000</v>
-      </c>
-      <c r="Q4">
-        <v>100000</v>
-      </c>
-      <c r="R4">
-        <v>100000</v>
-      </c>
-      <c r="S4">
-        <v>100000</v>
-      </c>
-      <c r="T4">
-        <v>100000</v>
-      </c>
-      <c r="U4">
-        <v>100000</v>
-      </c>
-      <c r="V4">
-        <v>100000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
       <c r="B5">
         <v>100000</v>
       </c>
@@ -785,6 +833,15 @@
       </c>
       <c r="V5">
         <v>100000</v>
+      </c>
+      <c r="W5">
+        <v>17000000</v>
+      </c>
+      <c r="X5">
+        <v>4000000</v>
+      </c>
+      <c r="Y5">
+        <v>10000000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>